<commit_message>
wrote 2 sections: last one was base ultimate
</commit_message>
<xml_diff>
--- a/Excel/Monsters_in_Games.xlsx
+++ b/Excel/Monsters_in_Games.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piercson\Desktop\Coding\Python\Monster Hunter\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37BB7B63-DE6A-4E50-BACB-8E05325C4CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1258B835-293C-4B8A-920D-573263374DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-4290" windowWidth="16440" windowHeight="28440" xr2:uid="{E347F027-0C1B-477F-B591-9CE3BB95789D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="296">
   <si>
     <t>Apceros</t>
   </si>
@@ -916,6 +916,12 @@
   </si>
   <si>
     <t>Monster Hunter X</t>
+  </si>
+  <si>
+    <t>Monster Hunter Portable 2nd</t>
+  </si>
+  <si>
+    <t>Monster Hunter Portable 2nd G</t>
   </si>
 </sst>
 </file>
@@ -1268,10 +1274,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B59A74B2-749B-409C-8E41-A018AD7404FB}">
-  <dimension ref="A1:S130"/>
+  <dimension ref="A1:U130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,9 +1301,11 @@
     <col min="17" max="17" width="31" customWidth="1"/>
     <col min="18" max="18" width="29.140625" customWidth="1"/>
     <col min="19" max="19" width="30.28515625" customWidth="1"/>
+    <col min="20" max="20" width="27.42578125" customWidth="1"/>
+    <col min="21" max="21" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -1355,8 +1363,14 @@
       <c r="S1" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>294</v>
+      </c>
+      <c r="U1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1414,8 +1428,14 @@
       <c r="S2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1473,8 +1493,14 @@
       <c r="S3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T3" t="s">
+        <v>53</v>
+      </c>
+      <c r="U3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1532,8 +1558,14 @@
       <c r="S4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T4" t="s">
+        <v>5</v>
+      </c>
+      <c r="U4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1591,8 +1623,14 @@
       <c r="S5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T5" t="s">
+        <v>58</v>
+      </c>
+      <c r="U5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1650,8 +1688,14 @@
       <c r="S6" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T6" t="s">
+        <v>10</v>
+      </c>
+      <c r="U6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1709,8 +1753,14 @@
       <c r="S7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T7" t="s">
+        <v>8</v>
+      </c>
+      <c r="U7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1768,8 +1818,14 @@
       <c r="S8" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T8" t="s">
+        <v>7</v>
+      </c>
+      <c r="U8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1827,8 +1883,14 @@
       <c r="S9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T9" t="s">
+        <v>59</v>
+      </c>
+      <c r="U9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1886,8 +1948,14 @@
       <c r="S10" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T10" t="s">
+        <v>50</v>
+      </c>
+      <c r="U10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1945,8 +2013,14 @@
       <c r="S11" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T11" t="s">
+        <v>9</v>
+      </c>
+      <c r="U11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2004,8 +2078,14 @@
       <c r="S12" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T12" t="s">
+        <v>55</v>
+      </c>
+      <c r="U12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2063,8 +2143,14 @@
       <c r="S13" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T13" t="s">
+        <v>12</v>
+      </c>
+      <c r="U13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -2122,8 +2208,14 @@
       <c r="S14" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T14" t="s">
+        <v>1</v>
+      </c>
+      <c r="U14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2181,8 +2273,14 @@
       <c r="S15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T15" t="s">
+        <v>3</v>
+      </c>
+      <c r="U15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -2240,8 +2338,14 @@
       <c r="S16" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T16" t="s">
+        <v>6</v>
+      </c>
+      <c r="U16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -2299,8 +2403,14 @@
       <c r="S17" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T17" t="s">
+        <v>0</v>
+      </c>
+      <c r="U17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -2358,8 +2468,14 @@
       <c r="S18" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T18" t="s">
+        <v>56</v>
+      </c>
+      <c r="U18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -2417,8 +2533,14 @@
       <c r="S19" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T19" t="s">
+        <v>51</v>
+      </c>
+      <c r="U19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -2476,8 +2598,14 @@
       <c r="S20" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T20" t="s">
+        <v>54</v>
+      </c>
+      <c r="U20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -2535,8 +2663,14 @@
       <c r="S21" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T21" t="s">
+        <v>57</v>
+      </c>
+      <c r="U21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -2594,8 +2728,14 @@
       <c r="S22" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T22" t="s">
+        <v>52</v>
+      </c>
+      <c r="U22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -2653,8 +2793,14 @@
       <c r="S23" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T23" t="s">
+        <v>11</v>
+      </c>
+      <c r="U23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -2712,8 +2858,14 @@
       <c r="S24" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T24" t="s">
+        <v>2</v>
+      </c>
+      <c r="U24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -2771,8 +2923,14 @@
       <c r="S25" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T25" t="s">
+        <v>75</v>
+      </c>
+      <c r="U25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -2830,8 +2988,14 @@
       <c r="S26" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T26" t="s">
+        <v>46</v>
+      </c>
+      <c r="U26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -2889,8 +3053,14 @@
       <c r="S27" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T27" t="s">
+        <v>23</v>
+      </c>
+      <c r="U27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -2948,8 +3118,14 @@
       <c r="S28" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T28" t="s">
+        <v>17</v>
+      </c>
+      <c r="U28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -3007,8 +3183,14 @@
       <c r="S29" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T29" t="s">
+        <v>76</v>
+      </c>
+      <c r="U29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -3066,8 +3248,14 @@
       <c r="S30" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T30" t="s">
+        <v>61</v>
+      </c>
+      <c r="U30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -3125,8 +3313,14 @@
       <c r="S31" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T31" t="s">
+        <v>28</v>
+      </c>
+      <c r="U31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>25</v>
       </c>
@@ -3181,8 +3375,14 @@
       <c r="S32" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="T32" t="s">
+        <v>29</v>
+      </c>
+      <c r="U32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>11</v>
       </c>
@@ -3237,8 +3437,14 @@
       <c r="S33" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="T33" t="s">
+        <v>25</v>
+      </c>
+      <c r="U33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>12</v>
       </c>
@@ -3293,8 +3499,14 @@
       <c r="S34" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="T34" t="s">
+        <v>18</v>
+      </c>
+      <c r="U34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>44</v>
       </c>
@@ -3349,8 +3561,14 @@
       <c r="S35" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="36" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="T35" t="s">
+        <v>33</v>
+      </c>
+      <c r="U35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>45</v>
       </c>
@@ -3405,8 +3623,14 @@
       <c r="S36" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="37" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="T36" t="s">
+        <v>35</v>
+      </c>
+      <c r="U36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>6</v>
       </c>
@@ -3458,8 +3682,14 @@
       <c r="S37" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="T37" t="s">
+        <v>77</v>
+      </c>
+      <c r="U37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>46</v>
       </c>
@@ -3511,8 +3741,14 @@
       <c r="S38" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="T38" t="s">
+        <v>62</v>
+      </c>
+      <c r="U38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>26</v>
       </c>
@@ -3564,8 +3800,14 @@
       <c r="S39" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="40" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="T39" t="s">
+        <v>67</v>
+      </c>
+      <c r="U39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>19</v>
       </c>
@@ -3617,8 +3859,14 @@
       <c r="S40" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="41" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="T40" t="s">
+        <v>32</v>
+      </c>
+      <c r="U40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>20</v>
       </c>
@@ -3667,8 +3915,14 @@
       <c r="S41" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="42" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="T41" t="s">
+        <v>16</v>
+      </c>
+      <c r="U41" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>17</v>
       </c>
@@ -3717,8 +3971,14 @@
       <c r="S42" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="43" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="T42" t="s">
+        <v>39</v>
+      </c>
+      <c r="U42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>44</v>
       </c>
@@ -3767,8 +4027,14 @@
       <c r="S43" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="44" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="T43" t="s">
+        <v>41</v>
+      </c>
+      <c r="U43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>14</v>
       </c>
@@ -3817,8 +4083,14 @@
       <c r="S44" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="45" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="T44" t="s">
+        <v>21</v>
+      </c>
+      <c r="U44" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>28</v>
       </c>
@@ -3867,8 +4139,14 @@
       <c r="S45" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="46" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="T45" t="s">
+        <v>14</v>
+      </c>
+      <c r="U45" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>27</v>
       </c>
@@ -3917,8 +4195,14 @@
       <c r="S46" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="47" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="T46" t="s">
+        <v>63</v>
+      </c>
+      <c r="U46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
         <v>71</v>
       </c>
@@ -3964,8 +4248,14 @@
       <c r="S47" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="T47" t="s">
+        <v>68</v>
+      </c>
+      <c r="U47" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
         <v>73</v>
       </c>
@@ -4011,8 +4301,14 @@
       <c r="S48" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="49" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T48" t="s">
+        <v>27</v>
+      </c>
+      <c r="U48" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
         <v>26</v>
       </c>
@@ -4058,8 +4354,14 @@
       <c r="S49" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="50" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T49" t="s">
+        <v>19</v>
+      </c>
+      <c r="U49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
         <v>38</v>
       </c>
@@ -4105,8 +4407,14 @@
       <c r="S50" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="51" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T50" t="s">
+        <v>24</v>
+      </c>
+      <c r="U50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
         <v>40</v>
       </c>
@@ -4152,8 +4460,14 @@
       <c r="S51" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="52" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T51" t="s">
+        <v>20</v>
+      </c>
+      <c r="U51" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
         <v>15</v>
       </c>
@@ -4199,8 +4513,14 @@
       <c r="S52" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="53" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T52" t="s">
+        <v>44</v>
+      </c>
+      <c r="U52" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
         <v>61</v>
       </c>
@@ -4246,8 +4566,14 @@
       <c r="S53" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="54" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T53" t="s">
+        <v>22</v>
+      </c>
+      <c r="U53" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
         <v>28</v>
       </c>
@@ -4293,8 +4619,14 @@
       <c r="S54" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="55" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T54" t="s">
+        <v>64</v>
+      </c>
+      <c r="U54" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
         <v>29</v>
       </c>
@@ -4340,8 +4672,14 @@
       <c r="S55" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="56" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T55" t="s">
+        <v>69</v>
+      </c>
+      <c r="U55" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
         <v>36</v>
       </c>
@@ -4384,8 +4722,14 @@
       <c r="S56" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="57" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T56" t="s">
+        <v>37</v>
+      </c>
+      <c r="U56" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="57" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
         <v>42</v>
       </c>
@@ -4428,8 +4772,14 @@
       <c r="S57" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="58" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T57" t="s">
+        <v>26</v>
+      </c>
+      <c r="U57" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
         <v>13</v>
       </c>
@@ -4472,8 +4822,14 @@
       <c r="S58" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="59" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T58" t="s">
+        <v>38</v>
+      </c>
+      <c r="U58" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
         <v>34</v>
       </c>
@@ -4516,8 +4872,14 @@
       <c r="S59" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="60" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T59" t="s">
+        <v>40</v>
+      </c>
+      <c r="U59" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
         <v>62</v>
       </c>
@@ -4560,8 +4922,14 @@
       <c r="S60" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="61" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T60" t="s">
+        <v>15</v>
+      </c>
+      <c r="U60" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
         <v>67</v>
       </c>
@@ -4604,8 +4972,14 @@
       <c r="S61" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="62" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T61" t="s">
+        <v>43</v>
+      </c>
+      <c r="U61" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="62" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
         <v>32</v>
       </c>
@@ -4645,8 +5019,14 @@
       <c r="S62" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="63" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T62" t="s">
+        <v>65</v>
+      </c>
+      <c r="U62" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="63" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
         <v>46</v>
       </c>
@@ -4686,8 +5066,14 @@
       <c r="S63" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="64" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T63" t="s">
+        <v>70</v>
+      </c>
+      <c r="U63" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="64" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
         <v>23</v>
       </c>
@@ -4727,8 +5113,14 @@
       <c r="S64" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="65" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T64" t="s">
+        <v>73</v>
+      </c>
+      <c r="U64" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="65" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
         <v>17</v>
       </c>
@@ -4768,8 +5160,14 @@
       <c r="S65" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="66" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T65" t="s">
+        <v>36</v>
+      </c>
+      <c r="U65" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="66" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
         <v>14</v>
       </c>
@@ -4809,8 +5207,14 @@
       <c r="S66" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="67" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T66" t="s">
+        <v>42</v>
+      </c>
+      <c r="U66" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="67" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
         <v>63</v>
       </c>
@@ -4850,8 +5254,14 @@
       <c r="S67" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="68" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T67" t="s">
+        <v>13</v>
+      </c>
+      <c r="U67" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="68" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
         <v>68</v>
       </c>
@@ -4891,8 +5301,14 @@
       <c r="S68" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="69" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T68" t="s">
+        <v>34</v>
+      </c>
+      <c r="U68" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="69" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
         <v>72</v>
       </c>
@@ -4932,8 +5348,14 @@
       <c r="S69" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="70" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T69" t="s">
+        <v>60</v>
+      </c>
+      <c r="U69" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="70" spans="4:21" x14ac:dyDescent="0.25">
       <c r="E70" t="s">
         <v>66</v>
       </c>
@@ -4970,8 +5392,14 @@
       <c r="S70" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="71" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T70" t="s">
+        <v>66</v>
+      </c>
+      <c r="U70" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="71" spans="4:21" x14ac:dyDescent="0.25">
       <c r="E71" t="s">
         <v>71</v>
       </c>
@@ -5008,8 +5436,14 @@
       <c r="S71" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="72" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T71" t="s">
+        <v>71</v>
+      </c>
+      <c r="U71" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="4:21" x14ac:dyDescent="0.25">
       <c r="F72" t="s">
         <v>21</v>
       </c>
@@ -5043,8 +5477,11 @@
       <c r="S72" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="73" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="U72" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="73" spans="4:21" x14ac:dyDescent="0.25">
       <c r="F73" t="s">
         <v>34</v>
       </c>
@@ -5078,8 +5515,11 @@
       <c r="S73" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="74" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="U73" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="74" spans="4:21" x14ac:dyDescent="0.25">
       <c r="F74" t="s">
         <v>77</v>
       </c>
@@ -5110,8 +5550,11 @@
       <c r="S74" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="75" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="U74" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="75" spans="4:21" x14ac:dyDescent="0.25">
       <c r="F75" t="s">
         <v>22</v>
       </c>
@@ -5139,8 +5582,11 @@
       <c r="S75" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="76" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="U75" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="4:21" x14ac:dyDescent="0.25">
       <c r="F76" t="s">
         <v>60</v>
       </c>
@@ -5168,8 +5614,11 @@
       <c r="S76" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="77" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="U76" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="4:21" x14ac:dyDescent="0.25">
       <c r="F77" t="s">
         <v>86</v>
       </c>
@@ -5197,8 +5646,11 @@
       <c r="S77" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="78" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="U77" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="78" spans="4:21" x14ac:dyDescent="0.25">
       <c r="F78" t="s">
         <v>64</v>
       </c>
@@ -5226,8 +5678,11 @@
       <c r="S78" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="79" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="U78" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="79" spans="4:21" x14ac:dyDescent="0.25">
       <c r="F79" t="s">
         <v>88</v>
       </c>
@@ -5255,8 +5710,11 @@
       <c r="S79" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="80" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="U79" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="80" spans="4:21" x14ac:dyDescent="0.25">
       <c r="F80" t="s">
         <v>28</v>
       </c>
@@ -5281,8 +5739,11 @@
       <c r="S80" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="81" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="U80" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="81" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F81" t="s">
         <v>69</v>
       </c>
@@ -5307,8 +5768,11 @@
       <c r="S81" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="82" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="U81" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="82" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F82" t="s">
         <v>29</v>
       </c>
@@ -5333,8 +5797,11 @@
       <c r="S82" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="83" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="U82" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="83" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F83" t="s">
         <v>27</v>
       </c>
@@ -5359,8 +5826,11 @@
       <c r="S83" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="84" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="U83" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="84" spans="6:21" x14ac:dyDescent="0.25">
       <c r="K84" t="s">
         <v>19</v>
       </c>
@@ -5383,7 +5853,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="85" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="85" spans="6:21" x14ac:dyDescent="0.25">
       <c r="K85" t="s">
         <v>133</v>
       </c>
@@ -5406,7 +5876,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="86" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="86" spans="6:21" x14ac:dyDescent="0.25">
       <c r="K86" t="s">
         <v>158</v>
       </c>
@@ -5429,7 +5899,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="87" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="87" spans="6:21" x14ac:dyDescent="0.25">
       <c r="K87" t="s">
         <v>41</v>
       </c>
@@ -5452,7 +5922,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="88" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="88" spans="6:21" x14ac:dyDescent="0.25">
       <c r="K88" t="s">
         <v>171</v>
       </c>
@@ -5475,7 +5945,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="89" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="89" spans="6:21" x14ac:dyDescent="0.25">
       <c r="K89" t="s">
         <v>174</v>
       </c>
@@ -5498,7 +5968,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="90" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="90" spans="6:21" x14ac:dyDescent="0.25">
       <c r="K90" t="s">
         <v>25</v>
       </c>
@@ -5521,7 +5991,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="91" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="91" spans="6:21" x14ac:dyDescent="0.25">
       <c r="K91" t="s">
         <v>175</v>
       </c>
@@ -5544,7 +6014,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="92" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="92" spans="6:21" x14ac:dyDescent="0.25">
       <c r="K92" t="s">
         <v>165</v>
       </c>
@@ -5567,7 +6037,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="93" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="93" spans="6:21" x14ac:dyDescent="0.25">
       <c r="K93" t="s">
         <v>177</v>
       </c>
@@ -5590,7 +6060,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="94" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="94" spans="6:21" x14ac:dyDescent="0.25">
       <c r="K94" t="s">
         <v>71</v>
       </c>
@@ -5613,7 +6083,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="95" spans="6:21" x14ac:dyDescent="0.25">
       <c r="K95" t="s">
         <v>178</v>
       </c>
@@ -5636,7 +6106,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="96" spans="6:21" x14ac:dyDescent="0.25">
       <c r="K96" t="s">
         <v>118</v>
       </c>

</xml_diff>